<commit_message>
updated schemas on PPT
</commit_message>
<xml_diff>
--- a/unchained-flight-insurance-web/bayesValidation.xlsx
+++ b/unchained-flight-insurance-web/bayesValidation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\git\unchained-flight-insurance\unchained-flight-insurance-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{ECC4613F-8499-4FEA-BAB5-9220ABCBACD4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AF19E917-6FBD-4C22-A10D-6E33FB1EBFE1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10233" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="9800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bayesValidation" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bayesValidation!$A$1:$D$558</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11685" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11685" uniqueCount="88">
   <si>
     <t>companyName</t>
   </si>
@@ -281,11 +281,20 @@
   <si>
     <t>cumulative number of flights [%]</t>
   </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2440,7 +2449,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ultimate</c:v>
+                  <c:v>Gold</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2448,7 +2457,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2551,7 +2560,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Medium</c:v>
+                  <c:v>Silver</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2559,7 +2568,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2662,7 +2671,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Basic</c:v>
+                  <c:v>Bronze</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2670,7 +2679,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -6862,7 +6871,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D3538"/>
   <sheetViews>
@@ -23628,7 +23637,7 @@
       <c r="B3538"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D558">
+  <autoFilter ref="A1:D558" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="EASYJET"/>
@@ -23643,7 +23652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3538"/>
   <sheetViews>
     <sheetView topLeftCell="A2697" workbookViewId="0">
@@ -73190,11 +73199,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -73519,13 +73528,13 @@
         <v>84</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.5">
@@ -73544,15 +73553,15 @@
         <v>0.44838343732274533</v>
       </c>
       <c r="F45" s="4">
-        <f>E$42*($C45*$E$37+$E$38)+$E$39</f>
+        <f t="shared" ref="F45:H55" si="0">E$42*($C45*$E$37+$E$38)+$E$39</f>
         <v>805</v>
       </c>
       <c r="G45" s="4">
-        <f>F$42*($C45*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>205</v>
       </c>
       <c r="H45" s="4">
-        <f>G$42*($C45*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
@@ -73568,15 +73577,15 @@
         <v>0.63528077141236527</v>
       </c>
       <c r="F46" s="4">
-        <f>E$42*($C46*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>1685.0000000000002</v>
       </c>
       <c r="G46" s="4">
-        <f>F$42*($C46*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>425.00000000000006</v>
       </c>
       <c r="H46" s="4">
-        <f>G$42*($C46*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>110.00000000000001</v>
       </c>
     </row>
@@ -73588,19 +73597,19 @@
         <v>560</v>
       </c>
       <c r="E47">
-        <f t="shared" ref="E47:E55" si="0">E46+D47/SUM(D$45:D$55)</f>
+        <f t="shared" ref="E47:E55" si="1">E46+D47/SUM(D$45:D$55)</f>
         <v>0.79410096426545662</v>
       </c>
       <c r="F47" s="4">
-        <f>E$42*($C47*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>2565.0000000000005</v>
       </c>
       <c r="G47" s="4">
-        <f>F$42*($C47*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>645.00000000000011</v>
       </c>
       <c r="H47" s="4">
-        <f>G$42*($C47*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>165.00000000000003</v>
       </c>
     </row>
@@ -73612,19 +73621,19 @@
         <v>365</v>
       </c>
       <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0.89761769710720363</v>
+      </c>
+      <c r="F48" s="4">
         <f t="shared" si="0"/>
-        <v>0.89761769710720363</v>
-      </c>
-      <c r="F48" s="4">
-        <f>E$42*($C48*$E$37+$E$38)+$E$39</f>
         <v>3445.0000000000005</v>
       </c>
       <c r="G48" s="4">
-        <f>F$42*($C48*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>865.00000000000011</v>
       </c>
       <c r="H48" s="4">
-        <f>G$42*($C48*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>220.00000000000003</v>
       </c>
     </row>
@@ -73636,19 +73645,19 @@
         <v>243</v>
       </c>
       <c r="E49">
+        <f t="shared" si="1"/>
+        <v>0.96653431650595578</v>
+      </c>
+      <c r="F49" s="4">
         <f t="shared" si="0"/>
-        <v>0.96653431650595578</v>
-      </c>
-      <c r="F49" s="4">
-        <f>E$42*($C49*$E$37+$E$38)+$E$39</f>
         <v>4325</v>
       </c>
       <c r="G49" s="4">
-        <f>F$42*($C49*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>1085</v>
       </c>
       <c r="H49" s="4">
-        <f>G$42*($C49*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>275</v>
       </c>
     </row>
@@ -73660,19 +73669,19 @@
         <v>70</v>
       </c>
       <c r="E50">
+        <f t="shared" si="1"/>
+        <v>0.98638684061259219</v>
+      </c>
+      <c r="F50" s="4">
         <f t="shared" si="0"/>
-        <v>0.98638684061259219</v>
-      </c>
-      <c r="F50" s="4">
-        <f>E$42*($C50*$E$37+$E$38)+$E$39</f>
         <v>5205</v>
       </c>
       <c r="G50" s="4">
-        <f>F$42*($C50*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>1305</v>
       </c>
       <c r="H50" s="4">
-        <f>G$42*($C50*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>330</v>
       </c>
     </row>
@@ -73684,19 +73693,19 @@
         <v>0</v>
       </c>
       <c r="E51">
+        <f t="shared" si="1"/>
+        <v>0.98638684061259219</v>
+      </c>
+      <c r="F51" s="4">
         <f t="shared" si="0"/>
-        <v>0.98638684061259219</v>
-      </c>
-      <c r="F51" s="4">
-        <f>E$42*($C51*$E$37+$E$38)+$E$39</f>
         <v>6085</v>
       </c>
       <c r="G51" s="4">
-        <f>F$42*($C51*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>1525</v>
       </c>
       <c r="H51" s="4">
-        <f>G$42*($C51*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>385</v>
       </c>
     </row>
@@ -73708,19 +73717,19 @@
         <v>27</v>
       </c>
       <c r="E52">
+        <f t="shared" si="1"/>
+        <v>0.99404424276800907</v>
+      </c>
+      <c r="F52" s="4">
         <f t="shared" si="0"/>
-        <v>0.99404424276800907</v>
-      </c>
-      <c r="F52" s="4">
-        <f>E$42*($C52*$E$37+$E$38)+$E$39</f>
         <v>6965</v>
       </c>
       <c r="G52" s="4">
-        <f>F$42*($C52*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>1745</v>
       </c>
       <c r="H52" s="4">
-        <f>G$42*($C52*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>440</v>
       </c>
     </row>
@@ -73732,19 +73741,19 @@
         <v>0</v>
       </c>
       <c r="E53">
+        <f t="shared" si="1"/>
+        <v>0.99404424276800907</v>
+      </c>
+      <c r="F53" s="4">
         <f t="shared" si="0"/>
-        <v>0.99404424276800907</v>
-      </c>
-      <c r="F53" s="4">
-        <f>E$42*($C53*$E$37+$E$38)+$E$39</f>
         <v>7845.0000000000009</v>
       </c>
       <c r="G53" s="4">
-        <f>F$42*($C53*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>1965.0000000000002</v>
       </c>
       <c r="H53" s="4">
-        <f>G$42*($C53*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>495.00000000000006</v>
       </c>
     </row>
@@ -73756,19 +73765,19 @@
         <v>0</v>
       </c>
       <c r="E54">
+        <f t="shared" si="1"/>
+        <v>0.99404424276800907</v>
+      </c>
+      <c r="F54" s="4">
         <f t="shared" si="0"/>
-        <v>0.99404424276800907</v>
-      </c>
-      <c r="F54" s="4">
-        <f>E$42*($C54*$E$37+$E$38)+$E$39</f>
         <v>8725</v>
       </c>
       <c r="G54" s="4">
-        <f>F$42*($C54*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>2185</v>
       </c>
       <c r="H54" s="4">
-        <f>G$42*($C54*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>550</v>
       </c>
     </row>
@@ -73783,19 +73792,19 @@
         <v>21</v>
       </c>
       <c r="E55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F55" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F55" s="4">
-        <f>E$42*($C55*$E$37+$E$38)+$E$39</f>
         <v>9605.0000000000018</v>
       </c>
       <c r="G55" s="4">
-        <f>F$42*($C55*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>2405.0000000000005</v>
       </c>
       <c r="H55" s="4">
-        <f>G$42*($C55*$E$37+$E$38)+$E$39</f>
+        <f t="shared" si="0"/>
         <v>605.00000000000011</v>
       </c>
     </row>

</xml_diff>